<commit_message>
utilized formulas and macros in sheets to solve problems for Excel-VBA assessment
</commit_message>
<xml_diff>
--- a/conditional_formatting.xlsx
+++ b/conditional_formatting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Travis\TrilogyCE\Module 2 Unit Assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyobu\Desktop\Analysis Projects\Excel-VBA-Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F769012-0727-4FCD-9F56-52D654D9DA96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F294543-D865-4D2B-BB8B-B53C565216DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{264DE790-16AF-460D-8D56-2179911DEA84}"/>
+    <workbookView xWindow="10755" yWindow="-11145" windowWidth="9600" windowHeight="4950" xr2:uid="{264DE790-16AF-460D-8D56-2179911DEA84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,111 +379,122 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>72</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>